<commit_message>
updates to make this more robust.
</commit_message>
<xml_diff>
--- a/distances_output.xlsx
+++ b/distances_output.xlsx
@@ -510,16 +510,16 @@
         <v>21</v>
       </c>
       <c r="C2">
-        <v>348.13</v>
+        <v>353.73</v>
       </c>
       <c r="D2">
-        <v>3.7</v>
+        <v>3.76</v>
       </c>
       <c r="E2">
-        <v>356.72</v>
+        <v>301.89</v>
       </c>
       <c r="F2">
-        <v>4.74</v>
+        <v>3.75</v>
       </c>
       <c r="G2">
         <v>345.47</v>
@@ -545,16 +545,16 @@
         <v>14</v>
       </c>
       <c r="C3">
-        <v>456.26</v>
+        <v>455.93</v>
       </c>
       <c r="D3">
-        <v>5.99</v>
+        <v>5.96</v>
       </c>
       <c r="E3">
         <v>500.88</v>
       </c>
       <c r="F3">
-        <v>2.43</v>
+        <v>2.48</v>
       </c>
       <c r="G3">
         <v>376.05</v>
@@ -609,10 +609,10 @@
         <v>5.5</v>
       </c>
       <c r="E5">
-        <v>532.27</v>
+        <v>532.22</v>
       </c>
       <c r="F5">
-        <v>3.45</v>
+        <v>3.47</v>
       </c>
       <c r="G5">
         <v>481.52</v>
@@ -679,7 +679,7 @@
         <v>8.93</v>
       </c>
       <c r="E7">
-        <v>946.5700000000001</v>
+        <v>941.36</v>
       </c>
       <c r="F7">
         <v>10.83</v>
@@ -714,10 +714,10 @@
         <v>5.35</v>
       </c>
       <c r="E8">
-        <v>538.21</v>
+        <v>526.5</v>
       </c>
       <c r="F8">
-        <v>5.55</v>
+        <v>6.58</v>
       </c>
       <c r="G8">
         <v>552.02</v>
@@ -749,10 +749,10 @@
         <v>6.33</v>
       </c>
       <c r="E9">
-        <v>785.45</v>
+        <v>785.46</v>
       </c>
       <c r="F9">
-        <v>5.68</v>
+        <v>6.35</v>
       </c>
       <c r="G9">
         <v>569.89</v>
@@ -784,7 +784,7 @@
         <v>12.34</v>
       </c>
       <c r="E10">
-        <v>1383.01</v>
+        <v>1383</v>
       </c>
       <c r="F10">
         <v>17.82</v>
@@ -819,10 +819,10 @@
         <v>1.53</v>
       </c>
       <c r="E11">
-        <v>137.8</v>
+        <v>147.34</v>
       </c>
       <c r="F11">
-        <v>1.48</v>
+        <v>2</v>
       </c>
       <c r="G11">
         <v>137.96</v>

</xml_diff>